<commit_message>
MASTER: Add new bayes results.
</commit_message>
<xml_diff>
--- a/doc/bayes.xlsx
+++ b/doc/bayes.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="11">
   <si>
     <t>Normalization function</t>
   </si>
@@ -43,6 +43,9 @@
   </si>
   <si>
     <t>F-measure</t>
+  </si>
+  <si>
+    <t>AUC</t>
   </si>
 </sst>
 </file>
@@ -88,16 +91,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:H31"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="21.5703125" customWidth="true"/>
     <col min="2" max="2" width="5.5703125" customWidth="true"/>
-    <col min="3" max="3" width="14.7109375" customWidth="true"/>
+    <col min="3" max="3" width="6.7109375" customWidth="true"/>
     <col min="4" max="4" width="12.7109375" customWidth="true"/>
     <col min="5" max="5" width="12.7109375" customWidth="true"/>
     <col min="6" max="6" width="12.7109375" customWidth="true"/>
     <col min="7" max="7" width="12.7109375" customWidth="true"/>
+    <col min="8" max="8" width="12.7109375" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -122,6 +126,9 @@
       <c r="G1" s="0" t="s">
         <v>9</v>
       </c>
+      <c r="H1" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
@@ -129,19 +136,22 @@
       </c>
       <c r="B2" s="0"/>
       <c r="C2" s="0">
-        <v>9.566037735849056</v>
+        <v>2699.5999999999999</v>
       </c>
       <c r="D2" s="0">
-        <v>0.62893081761006286</v>
+        <v>0.64737740533829924</v>
       </c>
       <c r="E2" s="0">
-        <v>0.33333333333333331</v>
+        <v>0.93549313358302122</v>
       </c>
       <c r="F2" s="0">
-        <v>0.65972222222222221</v>
+        <v>0.35923845193508119</v>
       </c>
       <c r="G2" s="0">
-        <v>0.76305220883534142</v>
+        <v>0.50352243136166175</v>
+      </c>
+      <c r="H2" s="0">
+        <v>0.64736579275905126</v>
       </c>
     </row>
     <row r="3">
@@ -150,19 +160,22 @@
       </c>
       <c r="B3" s="0"/>
       <c r="C3" s="0">
-        <v>0.056603773584905662</v>
+        <v>80.400000000000006</v>
       </c>
       <c r="D3" s="0">
-        <v>0.95597484276729561</v>
+        <v>0.91210117939168212</v>
       </c>
       <c r="E3" s="0">
-        <v>0.81818181818181823</v>
+        <v>0.86762796504369555</v>
       </c>
       <c r="F3" s="0">
-        <v>0.96621621621621623</v>
+        <v>0.956629213483146</v>
       </c>
       <c r="G3" s="0">
-        <v>0.97610921501706482</v>
+        <v>0.91599312731606375</v>
+      </c>
+      <c r="H3" s="0">
+        <v>0.91212858926342089</v>
       </c>
     </row>
     <row r="4">
@@ -171,19 +184,22 @@
       </c>
       <c r="B4" s="0"/>
       <c r="C4" s="0">
-        <v>25.761006289308177</v>
+        <v>2039.4000000000001</v>
       </c>
       <c r="D4" s="0">
-        <v>0.57232704402515722</v>
+        <v>0.68629112352576049</v>
       </c>
       <c r="E4" s="0">
-        <v>0.8666666666666667</v>
+        <v>0.93549313358302122</v>
       </c>
       <c r="F4" s="0">
-        <v>0.54166666666666663</v>
+        <v>0.43704119850187262</v>
       </c>
       <c r="G4" s="0">
-        <v>0.6964285714285714</v>
+        <v>0.57996404383954947</v>
+      </c>
+      <c r="H4" s="0">
+        <v>0.68626716604244709</v>
       </c>
     </row>
     <row r="5">
@@ -192,19 +208,22 @@
       </c>
       <c r="B5" s="0"/>
       <c r="C5" s="0">
-        <v>38.264150943396224</v>
+        <v>2591.8000000000002</v>
       </c>
       <c r="D5" s="0">
-        <v>0.47169811320754718</v>
+        <v>0.65517690875232781</v>
       </c>
       <c r="E5" s="0">
-        <v>0.84210526315789469</v>
+        <v>0.93769038701622986</v>
       </c>
       <c r="F5" s="0">
-        <v>0.42142857142857143</v>
+        <v>0.37267166042446942</v>
       </c>
       <c r="G5" s="0">
-        <v>0.58415841584158412</v>
+        <v>0.51869582032522388</v>
+      </c>
+      <c r="H5" s="0">
+        <v>0.65518102372034959</v>
       </c>
     </row>
     <row r="6">
@@ -213,19 +232,22 @@
       </c>
       <c r="B6" s="0"/>
       <c r="C6" s="0">
-        <v>41.264150943396224</v>
+        <v>2745.8000000000002</v>
       </c>
       <c r="D6" s="0">
-        <v>0.49056603773584906</v>
+        <v>0.65180633147113609</v>
       </c>
       <c r="E6" s="0">
-        <v>1</v>
+        <v>0.94220973782771544</v>
       </c>
       <c r="F6" s="0">
-        <v>0.4452054794520548</v>
+        <v>0.36144818976279652</v>
       </c>
       <c r="G6" s="0">
-        <v>0.61611374407582942</v>
+        <v>0.50847230149375533</v>
+      </c>
+      <c r="H6" s="0">
+        <v>0.6518289637952559</v>
       </c>
     </row>
     <row r="7">
@@ -234,19 +256,22 @@
       </c>
       <c r="B7" s="0"/>
       <c r="C7" s="0">
-        <v>3.9308176100628929</v>
+        <v>1740.0999999999999</v>
       </c>
       <c r="D7" s="0">
-        <v>0.76729559748427678</v>
+        <v>0.64277777777777789</v>
       </c>
       <c r="E7" s="0">
-        <v>0.59999999999999998</v>
+        <v>0.87333333333333329</v>
       </c>
       <c r="F7" s="0">
-        <v>0.78472222222222221</v>
+        <v>0.41222222222222216</v>
       </c>
       <c r="G7" s="0">
-        <v>0.85931558935361219</v>
+        <v>0.53567103225659896</v>
+      </c>
+      <c r="H7" s="0">
+        <v>0.64277777777777789</v>
       </c>
     </row>
     <row r="8">
@@ -255,19 +280,22 @@
       </c>
       <c r="B8" s="0"/>
       <c r="C8" s="0">
-        <v>0.3081761006289308</v>
+        <v>659.79999999999995</v>
       </c>
       <c r="D8" s="0">
-        <v>0.88050314465408808</v>
+        <v>0.78421787709497204</v>
       </c>
       <c r="E8" s="0">
-        <v>0.7142857142857143</v>
+        <v>0.92439450686641711</v>
       </c>
       <c r="F8" s="0">
-        <v>0.90579710144927539</v>
+        <v>0.64408239700374526</v>
       </c>
       <c r="G8" s="0">
-        <v>0.92936802973977695</v>
+        <v>0.74814851458377751</v>
+      </c>
+      <c r="H8" s="0">
+        <v>0.78423845193508113</v>
       </c>
     </row>
     <row r="9">
@@ -276,19 +304,22 @@
       </c>
       <c r="B9" s="0"/>
       <c r="C9" s="0">
-        <v>12.176100628930818</v>
+        <v>994.60000000000002</v>
       </c>
       <c r="D9" s="0">
-        <v>0.68553459119496851</v>
+        <v>0.76973929236499061</v>
       </c>
       <c r="E9" s="0">
-        <v>0.86363636363636365</v>
+        <v>0.94323345817727833</v>
       </c>
       <c r="F9" s="0">
-        <v>0.65693430656934304</v>
+        <v>0.59625468164794015</v>
       </c>
       <c r="G9" s="0">
-        <v>0.78260869565217395</v>
+        <v>0.72037182119388943</v>
+      </c>
+      <c r="H9" s="0">
+        <v>0.76974406991260913</v>
       </c>
     </row>
     <row r="10">
@@ -297,19 +328,22 @@
       </c>
       <c r="B10" s="0"/>
       <c r="C10" s="0">
-        <v>11.628930817610064</v>
+        <v>1394.3</v>
       </c>
       <c r="D10" s="0">
-        <v>0.67924528301886788</v>
+        <v>0.71134388578522667</v>
       </c>
       <c r="E10" s="0">
-        <v>0.76470588235294112</v>
+        <v>0.91774032459425725</v>
       </c>
       <c r="F10" s="0">
-        <v>0.66901408450704225</v>
+        <v>0.50495630461922603</v>
       </c>
       <c r="G10" s="0">
-        <v>0.7883817427385893</v>
+        <v>0.63529941905750453</v>
+      </c>
+      <c r="H10" s="0">
+        <v>0.71134831460674164</v>
       </c>
     </row>
     <row r="11">
@@ -318,19 +352,22 @@
       </c>
       <c r="B11" s="0"/>
       <c r="C11" s="0">
-        <v>37.289308176100626</v>
+        <v>2477.4000000000001</v>
       </c>
       <c r="D11" s="0">
-        <v>0.4779874213836478</v>
+        <v>0.60843575418994411</v>
       </c>
       <c r="E11" s="0">
-        <v>0.72727272727272729</v>
+        <v>0.88428214731585508</v>
       </c>
       <c r="F11" s="0">
-        <v>0.45945945945945948</v>
+        <v>0.33264669163545568</v>
       </c>
       <c r="G11" s="0">
-        <v>0.62100456621004563</v>
+        <v>0.45903742924697344</v>
+      </c>
+      <c r="H11" s="0">
+        <v>0.60846441947565544</v>
       </c>
     </row>
     <row r="12">
@@ -339,19 +376,22 @@
       </c>
       <c r="B12" s="0"/>
       <c r="C12" s="0">
-        <v>49.817610062893081</v>
+        <v>4519.3999999999996</v>
       </c>
       <c r="D12" s="0">
-        <v>0.33962264150943394</v>
+        <v>0.55506207324643075</v>
       </c>
       <c r="E12" s="0">
-        <v>0.63636363636363635</v>
+        <v>0.92771535580524345</v>
       </c>
       <c r="F12" s="0">
-        <v>0.29197080291970801</v>
+        <v>0.18247191011235955</v>
       </c>
       <c r="G12" s="0">
-        <v>0.4324324324324324</v>
+        <v>0.28833038339741912</v>
+      </c>
+      <c r="H12" s="0">
+        <v>0.55509363295880154</v>
       </c>
     </row>
     <row r="13">
@@ -360,19 +400,22 @@
       </c>
       <c r="B13" s="0"/>
       <c r="C13" s="0">
-        <v>0.3081761006289308</v>
+        <v>94.099999999999994</v>
       </c>
       <c r="D13" s="0">
-        <v>0.9308176100628931</v>
+        <v>0.9115642458100558</v>
       </c>
       <c r="E13" s="0">
-        <v>0.83333333333333337</v>
+        <v>0.86205992509363294</v>
       </c>
       <c r="F13" s="0">
-        <v>0.93877551020408168</v>
+        <v>0.96108614232209744</v>
       </c>
       <c r="G13" s="0">
-        <v>0.9616724738675958</v>
+        <v>0.9157619204511549</v>
+      </c>
+      <c r="H13" s="0">
+        <v>0.91157303370786524</v>
       </c>
     </row>
     <row r="14">
@@ -381,19 +424,22 @@
       </c>
       <c r="B14" s="0"/>
       <c r="C14" s="0">
-        <v>45.440251572327043</v>
+        <v>2738.9000000000001</v>
       </c>
       <c r="D14" s="0">
-        <v>0.44025157232704404</v>
+        <v>0.61678150217256356</v>
       </c>
       <c r="E14" s="0">
-        <v>0.8666666666666667</v>
+        <v>0.906541822721598</v>
       </c>
       <c r="F14" s="0">
-        <v>0.39583333333333331</v>
+        <v>0.32697877652933832</v>
       </c>
       <c r="G14" s="0">
-        <v>0.56157635467980294</v>
+        <v>0.45960931754896917</v>
+      </c>
+      <c r="H14" s="0">
+        <v>0.61676029962546808</v>
       </c>
     </row>
     <row r="15">
@@ -402,19 +448,22 @@
       </c>
       <c r="B15" s="0"/>
       <c r="C15" s="0">
-        <v>42.289308176100626</v>
+        <v>2379.6999999999998</v>
       </c>
       <c r="D15" s="0">
-        <v>0.47169811320754718</v>
+        <v>0.66131905648665434</v>
       </c>
       <c r="E15" s="0">
-        <v>0.94117647058823528</v>
+        <v>0.92993757802746568</v>
       </c>
       <c r="F15" s="0">
-        <v>0.41549295774647887</v>
+        <v>0.39275905118601739</v>
       </c>
       <c r="G15" s="0">
-        <v>0.58415841584158412</v>
+        <v>0.53382979881543136</v>
+      </c>
+      <c r="H15" s="0">
+        <v>0.66134831460674159</v>
       </c>
     </row>
     <row r="16">
@@ -423,19 +472,22 @@
       </c>
       <c r="B16" s="0"/>
       <c r="C16" s="0">
-        <v>36.327044025157235</v>
+        <v>2258.3000000000002</v>
       </c>
       <c r="D16" s="0">
-        <v>0.50943396226415094</v>
+        <v>0.67019553072625704</v>
       </c>
       <c r="E16" s="0">
-        <v>0.94117647058823528</v>
+        <v>0.9332958801498128</v>
       </c>
       <c r="F16" s="0">
-        <v>0.45774647887323944</v>
+        <v>0.40712858926342071</v>
       </c>
       <c r="G16" s="0">
-        <v>0.625</v>
+        <v>0.55129643934317085</v>
+      </c>
+      <c r="H16" s="0">
+        <v>0.67021223470661684</v>
       </c>
     </row>
     <row r="17">
@@ -444,19 +496,22 @@
       </c>
       <c r="B17" s="0"/>
       <c r="C17" s="0">
-        <v>32.60377358490566</v>
+        <v>3094.5</v>
       </c>
       <c r="D17" s="0">
-        <v>0.42138364779874216</v>
+        <v>0.59833333333333327</v>
       </c>
       <c r="E17" s="0">
-        <v>0.47368421052631576</v>
+        <v>0.90444444444444438</v>
       </c>
       <c r="F17" s="0">
-        <v>0.41428571428571431</v>
+        <v>0.29222222222222227</v>
       </c>
       <c r="G17" s="0">
-        <v>0.55769230769230771</v>
+        <v>0.41751705834148878</v>
+      </c>
+      <c r="H17" s="0">
+        <v>0.59833333333333327</v>
       </c>
     </row>
     <row r="18">
@@ -465,19 +520,22 @@
       </c>
       <c r="B18" s="0"/>
       <c r="C18" s="0">
-        <v>2.0377358490566038</v>
+        <v>4338.1999999999998</v>
       </c>
       <c r="D18" s="0">
-        <v>0.86163522012578619</v>
+        <v>0.60844506517690866</v>
       </c>
       <c r="E18" s="0">
-        <v>0.81818181818181823</v>
+        <v>0.97439450686641715</v>
       </c>
       <c r="F18" s="0">
-        <v>0.86486486486486491</v>
+        <v>0.24247191011235958</v>
       </c>
       <c r="G18" s="0">
-        <v>0.92086330935251803</v>
+        <v>0.38141999019705369</v>
+      </c>
+      <c r="H18" s="0">
+        <v>0.6084332084893882</v>
       </c>
     </row>
     <row r="19">
@@ -486,19 +544,22 @@
       </c>
       <c r="B19" s="0"/>
       <c r="C19" s="0">
-        <v>11.09433962264151</v>
+        <v>549.29999999999995</v>
       </c>
       <c r="D19" s="0">
-        <v>0.73584905660377353</v>
+        <v>0.83815021725636252</v>
       </c>
       <c r="E19" s="0">
-        <v>1</v>
+        <v>0.96554307116104887</v>
       </c>
       <c r="F19" s="0">
-        <v>0.71034482758620687</v>
+        <v>0.71071161048689147</v>
       </c>
       <c r="G19" s="0">
-        <v>0.83064516129032262</v>
+        <v>0.81384987256700703</v>
+      </c>
+      <c r="H19" s="0">
+        <v>0.83812734082397</v>
       </c>
     </row>
     <row r="20">
@@ -507,19 +568,22 @@
       </c>
       <c r="B20" s="0"/>
       <c r="C20" s="0">
-        <v>21.89308176100629</v>
+        <v>1614</v>
       </c>
       <c r="D20" s="0">
-        <v>0.5911949685534591</v>
+        <v>0.71967411545623849</v>
       </c>
       <c r="E20" s="0">
-        <v>0.83333333333333337</v>
+        <v>0.93993757802746569</v>
       </c>
       <c r="F20" s="0">
-        <v>0.56028368794326244</v>
+        <v>0.49947565543071165</v>
       </c>
       <c r="G20" s="0">
-        <v>0.70852017937219725</v>
+        <v>0.6386168840616967</v>
+      </c>
+      <c r="H20" s="0">
+        <v>0.71970661672908864</v>
       </c>
     </row>
     <row r="21">
@@ -528,19 +592,22 @@
       </c>
       <c r="B21" s="0"/>
       <c r="C21" s="0">
-        <v>42.289308176100626</v>
+        <v>3127.3000000000002</v>
       </c>
       <c r="D21" s="0">
-        <v>0.44654088050314467</v>
+        <v>0.62682184978274358</v>
       </c>
       <c r="E21" s="0">
-        <v>0.7857142857142857</v>
+        <v>0.93661672908863935</v>
       </c>
       <c r="F21" s="0">
-        <v>0.41379310344827586</v>
+        <v>0.31695380774032461</v>
       </c>
       <c r="G21" s="0">
-        <v>0.57692307692307687</v>
+        <v>0.45826849405554781</v>
+      </c>
+      <c r="H21" s="0">
+        <v>0.6267852684144819</v>
       </c>
     </row>
     <row r="22">
@@ -549,19 +616,22 @@
       </c>
       <c r="B22" s="0"/>
       <c r="C22" s="0">
-        <v>45.440251572327043</v>
+        <v>3807.6999999999998</v>
       </c>
       <c r="D22" s="0">
-        <v>0.42767295597484278</v>
+        <v>0.57232153941651143</v>
       </c>
       <c r="E22" s="0">
-        <v>0.80000000000000004</v>
+        <v>0.91440699126092395</v>
       </c>
       <c r="F22" s="0">
-        <v>0.3888888888888889</v>
+        <v>0.23028714107365794</v>
       </c>
       <c r="G22" s="0">
-        <v>0.55172413793103448</v>
+        <v>0.34870695852499489</v>
+      </c>
+      <c r="H22" s="0">
+        <v>0.57234706616729081</v>
       </c>
     </row>
     <row r="23">
@@ -570,19 +640,22 @@
       </c>
       <c r="B23" s="0"/>
       <c r="C23" s="0">
-        <v>0.0062893081761006293</v>
+        <v>131.90000000000001</v>
       </c>
       <c r="D23" s="0">
-        <v>0.94339622641509435</v>
+        <v>0.87817504655493495</v>
       </c>
       <c r="E23" s="0">
-        <v>0.77777777777777779</v>
+        <v>0.81978776529338315</v>
       </c>
       <c r="F23" s="0">
-        <v>0.96453900709219853</v>
+        <v>0.93654182272159792</v>
       </c>
       <c r="G23" s="0">
-        <v>0.9679715302491102</v>
+        <v>0.88473300809197486</v>
+      </c>
+      <c r="H23" s="0">
+        <v>0.87816479400749059</v>
       </c>
     </row>
     <row r="24">
@@ -591,19 +664,22 @@
       </c>
       <c r="B24" s="0"/>
       <c r="C24" s="0">
-        <v>37.289308176100626</v>
+        <v>2094.9000000000001</v>
       </c>
       <c r="D24" s="0">
-        <v>0.49056603773584906</v>
+        <v>0.65350403476101793</v>
       </c>
       <c r="E24" s="0">
-        <v>0.88888888888888884</v>
+        <v>0.90660424469413248</v>
       </c>
       <c r="F24" s="0">
-        <v>0.43971631205673761</v>
+        <v>0.40037453183520599</v>
       </c>
       <c r="G24" s="0">
-        <v>0.60487804878048779</v>
+        <v>0.53457705261663979</v>
+      </c>
+      <c r="H24" s="0">
+        <v>0.65348938826466918</v>
       </c>
     </row>
     <row r="25">
@@ -612,19 +688,22 @@
       </c>
       <c r="B25" s="0"/>
       <c r="C25" s="0">
-        <v>36.327044025157235</v>
+        <v>2412.8000000000002</v>
       </c>
       <c r="D25" s="0">
-        <v>0.50943396226415094</v>
+        <v>0.66959342023587842</v>
       </c>
       <c r="E25" s="0">
-        <v>0.90909090909090906</v>
+        <v>0.94212234706616726</v>
       </c>
       <c r="F25" s="0">
-        <v>0.47972972972972971</v>
+        <v>0.39711610486891386</v>
       </c>
       <c r="G25" s="0">
-        <v>0.64545454545454539</v>
+        <v>0.5448173463924032</v>
+      </c>
+      <c r="H25" s="0">
+        <v>0.66961922596754064</v>
       </c>
     </row>
     <row r="26">
@@ -633,19 +712,22 @@
       </c>
       <c r="B26" s="0"/>
       <c r="C26" s="0">
-        <v>35.377358490566039</v>
+        <v>2084.5999999999999</v>
       </c>
       <c r="D26" s="0">
-        <v>0.50314465408805031</v>
+        <v>0.66631284916201117</v>
       </c>
       <c r="E26" s="0">
-        <v>0.88235294117647056</v>
+        <v>0.91878901373283406</v>
       </c>
       <c r="F26" s="0">
-        <v>0.45774647887323944</v>
+        <v>0.41379525593008742</v>
       </c>
       <c r="G26" s="0">
-        <v>0.62200956937799046</v>
+        <v>0.5519961896031772</v>
+      </c>
+      <c r="H26" s="0">
+        <v>0.66629213483146077</v>
       </c>
     </row>
     <row r="27">
@@ -654,19 +736,22 @@
       </c>
       <c r="B27" s="0"/>
       <c r="C27" s="0">
-        <v>43.327044025157235</v>
+        <v>2946</v>
       </c>
       <c r="D27" s="0">
-        <v>0.41509433962264153</v>
+        <v>0.57666666666666655</v>
       </c>
       <c r="E27" s="0">
-        <v>0.54545454545454541</v>
+        <v>0.87777777777777788</v>
       </c>
       <c r="F27" s="0">
-        <v>0.40540540540540543</v>
+        <v>0.27555555555555555</v>
       </c>
       <c r="G27" s="0">
-        <v>0.56338028169014087</v>
+        <v>0.39345901727968574</v>
+      </c>
+      <c r="H27" s="0">
+        <v>0.57666666666666655</v>
       </c>
     </row>
     <row r="28">
@@ -675,19 +760,22 @@
       </c>
       <c r="B28" s="0"/>
       <c r="C28" s="0">
-        <v>0.025157232704402517</v>
+        <v>1710</v>
       </c>
       <c r="D28" s="0">
-        <v>0.96226415094339623</v>
+        <v>0.6907697082557418</v>
       </c>
       <c r="E28" s="0">
-        <v>0.59999999999999998</v>
+        <v>0.91097378277153562</v>
       </c>
       <c r="F28" s="0">
-        <v>0.98657718120805371</v>
+        <v>0.47049937578027468</v>
       </c>
       <c r="G28" s="0">
-        <v>0.97999999999999998</v>
+        <v>0.59601714987287135</v>
+      </c>
+      <c r="H28" s="0">
+        <v>0.69073657927590515</v>
       </c>
     </row>
     <row r="29">
@@ -696,19 +784,22 @@
       </c>
       <c r="B29" s="0"/>
       <c r="C29" s="0">
-        <v>12.176100628930818</v>
+        <v>880.5</v>
       </c>
       <c r="D29" s="0">
-        <v>0.71069182389937102</v>
+        <v>0.79813469894475486</v>
       </c>
       <c r="E29" s="0">
-        <v>0.94736842105263153</v>
+        <v>0.96108614232209733</v>
       </c>
       <c r="F29" s="0">
-        <v>0.6785714285714286</v>
+        <v>0.63516853932584272</v>
       </c>
       <c r="G29" s="0">
-        <v>0.80508474576271194</v>
+        <v>0.75810812728863097</v>
+      </c>
+      <c r="H29" s="0">
+        <v>0.79812734082397008</v>
       </c>
     </row>
     <row r="30">
@@ -717,19 +808,22 @@
       </c>
       <c r="B30" s="0"/>
       <c r="C30" s="0">
-        <v>23.40251572327044</v>
+        <v>1746.8</v>
       </c>
       <c r="D30" s="0">
-        <v>0.57861635220125784</v>
+        <v>0.70970515207945373</v>
       </c>
       <c r="E30" s="0">
-        <v>0.8125</v>
+        <v>0.94109862671660438</v>
       </c>
       <c r="F30" s="0">
-        <v>0.55244755244755239</v>
+        <v>0.47836454431960052</v>
       </c>
       <c r="G30" s="0">
-        <v>0.70222222222222208</v>
+        <v>0.62235015793752813</v>
+      </c>
+      <c r="H30" s="0">
+        <v>0.70973158551810245</v>
       </c>
     </row>
     <row r="31">
@@ -738,19 +832,22 @@
       </c>
       <c r="B31" s="0"/>
       <c r="C31" s="0">
-        <v>35.377358490566039</v>
+        <v>2760.5999999999999</v>
       </c>
       <c r="D31" s="0">
-        <v>0.45283018867924529</v>
+        <v>0.62179702048417129</v>
       </c>
       <c r="E31" s="0">
-        <v>0.75</v>
+        <v>0.91323345817727852</v>
       </c>
       <c r="F31" s="0">
-        <v>0.40000000000000002</v>
+        <v>0.33033707865168538</v>
       </c>
       <c r="G31" s="0">
-        <v>0.55384615384615388</v>
+        <v>0.46489525789444242</v>
+      </c>
+      <c r="H31" s="0">
+        <v>0.62178526841448201</v>
       </c>
     </row>
   </sheetData>

</xml_diff>